<commit_message>
Added EyeLink and Optotrak recording (still testing)
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vision Lab\Development\ShapeTapper\Config_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visionlab\Development\ShapeTapper\Manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>block_num</t>
   </si>
@@ -156,12 +156,6 @@
     <t>maximum time before trial times out</t>
   </si>
   <si>
-    <t>toggles trial end message (correct or not, etc)</t>
-  </si>
-  <si>
-    <t>name of image file (typically in the "Images/" subfolder</t>
-  </si>
-  <si>
     <t>duration that stimulus image is displayed onscreen</t>
   </si>
   <si>
@@ -171,12 +165,6 @@
     <t>stimulus rotation</t>
   </si>
   <si>
-    <t>0 = not target, 1 = gaze target, 2 = touch target</t>
-  </si>
-  <si>
-    <t>0 = not a fixation object, 1 = gaze fixation, 2 = touch fixation</t>
-  </si>
-  <si>
     <t>stimulus onset time (from trial start time, EXCLUDING fixation pauses)</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
     <t>margin of mask points around stim image</t>
   </si>
   <si>
-    <t>0 = not touchable, 1 = touchable</t>
-  </si>
-  <si>
     <t>stim_is_touchable</t>
   </si>
   <si>
@@ -222,16 +207,49 @@
     <t>background_color</t>
   </si>
   <si>
-    <t>can use "black" or "white" Default = white</t>
-  </si>
-  <si>
-    <t>color name</t>
+    <t>0 = not target, 1 = touch target, 2 =  gaze target</t>
+  </si>
+  <si>
+    <t>0 = not a fixation object, 1 = touch fixation, 2 = gaze fixation</t>
+  </si>
+  <si>
+    <t>examples:  "0 0 0" = black, "1 1 1" = white, "0.5 0.5 0.5" = grey, "1 0 0" = red, etc. [default = white]</t>
+  </si>
+  <si>
+    <t>0 = not touchable, 1 = touch only, 2 = gaze only,  3 = touch or gaze, 4 = touch and gaze</t>
+  </si>
+  <si>
+    <t>image file name, or "msg" which will display the message specified at the beginning of the script</t>
+  </si>
+  <si>
+    <t>trial_kb_resp</t>
+  </si>
+  <si>
+    <t>0 = no keyboard response, 1 = prompt for keyboard response at trial end</t>
+  </si>
+  <si>
+    <t>trial_timeout_msg</t>
+  </si>
+  <si>
+    <t>0=no timeout message, 1 = display timeout message if trial ends with no response</t>
+  </si>
+  <si>
+    <t>RGB (0-1)</t>
+  </si>
+  <si>
+    <t>text_color</t>
+  </si>
+  <si>
+    <t>examples:  "0 0 0" = black, "1 1 1" = white, "0.5 0.5 0.5" = grey, "1 0 0" = red, etc. [default = black]</t>
+  </si>
+  <si>
+    <t>name of image file (typically in the "Images/" subfolder)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1033,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1166,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1157,26 +1175,26 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
@@ -1185,194 +1203,194 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
@@ -1381,77 +1399,119 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
         <v>37</v>
       </c>
-      <c r="D29" t="s">
-        <v>61</v>
+      <c r="D32" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to fit config format changes
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>block_num</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>name of image file (typically in the "Images/" subfolder)</t>
+  </si>
+  <si>
+    <t>correct_kb_resp</t>
+  </si>
+  <si>
+    <t>a-z</t>
+  </si>
+  <si>
+    <t>set to "None" for default (if trial_kb_resp = 0)</t>
+  </si>
+  <si>
+    <t>trial_feedback_type</t>
+  </si>
+  <si>
+    <t>0 = no trial feedback, 1 = display trial feedback</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D10" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,189 +1209,189 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -1385,40 +1400,40 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
@@ -1427,12 +1442,12 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
@@ -1441,76 +1456,104 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D34" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed trial feedback config names and args
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -39,9 +39,6 @@
     <t>trial_max_time</t>
   </si>
   <si>
-    <t>trial_feedback</t>
-  </si>
-  <si>
     <t>stim_img_name</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>0 = not touchable, 1 = touch only, 2 = gaze only,  3 = touch or gaze, 4 = touch and gaze</t>
   </si>
   <si>
-    <t>image file name, or "msg" which will display the message specified at the beginning of the script</t>
-  </si>
-  <si>
     <t>trial_kb_resp</t>
   </si>
   <si>
@@ -258,7 +252,13 @@
     <t>trial_feedback_type</t>
   </si>
   <si>
-    <t>0 = no trial feedback, 1 = display trial feedback</t>
+    <t>0 = no trial feedback, 1 = display trial feedback, 2 = dislpay trial default message</t>
+  </si>
+  <si>
+    <t>trial_feedback_image</t>
+  </si>
+  <si>
+    <t>image file name</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,16 +1083,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,13 +1100,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,13 +1114,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,13 +1128,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,13 +1142,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,13 +1156,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,69 +1170,69 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
         <v>75</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,321 +1240,321 @@
         <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed trial_feedback naming in config file
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visionlab\Development\ShapeTapper\Manuals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vision Lab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="test_exp2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>block_num</t>
   </si>
@@ -153,18 +153,12 @@
     <t>maximum time before trial times out</t>
   </si>
   <si>
-    <t>duration that stimulus image is displayed onscreen</t>
-  </si>
-  <si>
     <t>stimulus actual size on screen</t>
   </si>
   <si>
     <t>stimulus rotation</t>
   </si>
   <si>
-    <t>stimulus onset time (from trial start time, EXCLUDING fixation pauses)</t>
-  </si>
-  <si>
     <t>fixation onset time (from trial start time, INCLUDING fixation pauses)</t>
   </si>
   <si>
@@ -252,19 +246,28 @@
     <t>trial_feedback_type</t>
   </si>
   <si>
-    <t>0 = no trial feedback, 1 = display trial feedback, 2 = dislpay trial default message</t>
-  </si>
-  <si>
-    <t>trial_feedback_image</t>
-  </si>
-  <si>
-    <t>image file name</t>
+    <t>Field Number</t>
+  </si>
+  <si>
+    <t>trial_feedback_img</t>
+  </si>
+  <si>
+    <t>image file name. Set to "None" for default if no image is required.</t>
+  </si>
+  <si>
+    <t>0 = no trial feedback, 1 = display trial feedback message</t>
+  </si>
+  <si>
+    <t>stimulus onset time (from trial start time, EXCLUDING fixation pauses). Codes for stim to appear based on gaze_ or touch_fixation dependences (-1 touch liftoff dependent; -2 gaze 'liftoff' dependent)</t>
+  </si>
+  <si>
+    <t>duration that stimulus image is displayed onscreen. Codes accepted for gaze or touch fixation dependencies (-1=touch liftoff dependent; -2=gaze 'liftoff' dependent; -3=remaining trial time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,7 +404,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +582,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -742,9 +751,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1066,495 +1077,598 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="174" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
       <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E34" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed fixations (optional pauses), stim onsets and durations
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vision Lab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visionlab\Development\ShapeTapper\Manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="10725"/>
   </bookViews>
   <sheets>
     <sheet name="test_exp2" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>block_num</t>
   </si>
@@ -262,12 +262,18 @@
   </si>
   <si>
     <t>duration that stimulus image is displayed onscreen. Codes accepted for gaze or touch fixation dependencies (-1=touch liftoff dependent; -2=gaze 'liftoff' dependent; -3=remaining trial time)</t>
+  </si>
+  <si>
+    <t>subj_fixation_pause</t>
+  </si>
+  <si>
+    <t>0=no fixation pause, 1=pause on current frame until fixation duration is satisfied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,7 +410,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,12 +588,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -751,10 +751,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1077,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1266,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C11" t="s">
@@ -1276,7 +1275,7 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1284,7 +1283,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C12" t="s">
@@ -1293,7 +1292,7 @@
       <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1518,21 +1517,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1540,7 +1539,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
@@ -1549,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,7 +1556,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
@@ -1566,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,7 +1573,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
@@ -1583,7 +1582,7 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,16 +1590,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1608,16 +1607,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,16 +1624,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1642,16 +1641,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,15 +1658,32 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
         <v>36</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Current version running participants Feb 2019
</commit_message>
<xml_diff>
--- a/Manuals/config_file_format.xlsx
+++ b/Manuals/config_file_format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visionlab\Development\ShapeTapper\Manuals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\Desktop\Shape Spider\Manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="test_exp2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -198,9 +198,6 @@
     <t>background_color</t>
   </si>
   <si>
-    <t>0 = not target, 1 = touch target, 2 =  gaze target</t>
-  </si>
-  <si>
     <t>0 = not a fixation object, 1 = touch fixation, 2 = gaze fixation</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>trial_kb_resp</t>
   </si>
   <si>
-    <t>0 = no keyboard response, 1 = prompt for keyboard response at trial end</t>
-  </si>
-  <si>
     <t>trial_timeout_msg</t>
   </si>
   <si>
@@ -268,6 +262,12 @@
   </si>
   <si>
     <t>0=no fixation pause, 1=pause on current frame until fixation duration is satisfied</t>
+  </si>
+  <si>
+    <t>0 = not target, 1 = touch target, 2 =  gaze target,  3 = touch or gaze target, 4 = touch and gaze target</t>
+  </si>
+  <si>
+    <t>0 = no keyboard response; 1 = prompt for keyboard response at trial end; 2 = end trial upon keyboard response, save key as user response; 3 = end trial upon keyboard response, then prompt for keyboard response at trial end</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>26</v>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
@@ -1225,7 +1225,7 @@
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -1242,7 +1242,7 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1250,16 +1250,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1276,7 +1276,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
@@ -1293,7 +1293,7 @@
         <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,10 +1307,10 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1318,16 +1318,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
         <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1522,7 +1522,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
@@ -1531,7 +1531,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>